<commit_message>
20-Feb-2017-2045 - Committing Changes of Client User along with the xlsx and .Java Files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/CDR Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/CDR Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>TCID</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Mobile Communications</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Automobiles &amp; Components;
 Banking</t>
   </si>
@@ -213,13 +210,16 @@
     <t>United States Dollar (USD)</t>
   </si>
   <si>
+    <t>CDRWorkflow</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>CDRWorkflow</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -677,22 +677,22 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -733,9 +733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -898,7 +898,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AE2" s="7"/>
     </row>
@@ -913,7 +913,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>31</v>
@@ -934,7 +934,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>52</v>
@@ -955,7 +955,7 @@
         <v>32</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S3" s="2">
         <v>1234567</v>
@@ -991,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AE3" s="6"/>
     </row>

</xml_diff>